<commit_message>
swapped zero cross pin for EXTI_2 line, HS1 recalculation
</commit_message>
<xml_diff>
--- a/documentation/pins.xlsx
+++ b/documentation/pins.xlsx
@@ -7,6 +7,11 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FfMG5PW5jfwh4rC7SOymaAgea0mmUjDbV6eZq+6Ov3Q="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -196,10 +201,10 @@
     <t>I_SENSE</t>
   </si>
   <si>
-    <t>PB2</t>
-  </si>
-  <si>
-    <t>ADC_IN10</t>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>ADC_IN16</t>
   </si>
   <si>
     <t>Heat lamp current sensor output, analog signal from 0 -&gt; vcc/2 (0A) -&gt;vcc.</t>
@@ -208,7 +213,7 @@
     <t>ZERO_CROSS</t>
   </si>
   <si>
-    <t>PB5</t>
+    <t>PD2</t>
   </si>
   <si>
     <t>Live/mains signal for sine wave zero cross detection (triac shut off point).</t>
@@ -424,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -438,9 +443,6 @@
     <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -976,10 +978,10 @@
       <c r="B18" s="6">
         <v>24.0</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E18" s="7" t="s">
@@ -990,10 +992,10 @@
       <c r="A19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="6">
-        <v>44.0</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="8">
+        <v>40.0</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="6" t="s">

</xml_diff>

<commit_message>
OLED driver, idle task, refactoring
</commit_message>
<xml_diff>
--- a/documentation/pins.xlsx
+++ b/documentation/pins.xlsx
@@ -57,28 +57,28 @@
     <t>I2C1</t>
   </si>
   <si>
+    <t>Temp &amp; humidity sensor  B I2C data signal.</t>
+  </si>
+  <si>
+    <t>I2C2_SCL</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>I2C2</t>
+  </si>
+  <si>
+    <t>Temp &amp; humidity sensor A I2C clock signal.</t>
+  </si>
+  <si>
+    <t>I2C2_SDA</t>
+  </si>
+  <si>
+    <t>PA12</t>
+  </si>
+  <si>
     <t>Temp &amp; humidity sensor  A I2C data signal.</t>
-  </si>
-  <si>
-    <t>I2C2_SCL</t>
-  </si>
-  <si>
-    <t>PA11</t>
-  </si>
-  <si>
-    <t>I2C2</t>
-  </si>
-  <si>
-    <t>Temp &amp; humidity sensor A I2C clock signal.</t>
-  </si>
-  <si>
-    <t>I2C2_SDA</t>
-  </si>
-  <si>
-    <t>PA12</t>
-  </si>
-  <si>
-    <t>Temp &amp; humidity sensor  B I2C data signal.</t>
   </si>
   <si>
     <t>DISP_MOSI</t>
@@ -429,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -443,6 +443,9 @@
     <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -743,10 +746,10 @@
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -780,7 +783,7 @@
       <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -995,7 +998,7 @@
       <c r="B19" s="8">
         <v>40.0</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="6" t="s">

</xml_diff>